<commit_message>
Updated successfully alert messages in all the tabes
</commit_message>
<xml_diff>
--- a/ExcelData/TC_AssetsTypes.xlsx
+++ b/ExcelData/TC_AssetsTypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23340" windowHeight="3615"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23370" windowHeight="10740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,13 @@
     <t>assetTypeDescription</t>
   </si>
   <si>
-    <t>GSR</t>
-  </si>
-  <si>
-    <t>Geyser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electric geyser </t>
+    <t>TabelFan</t>
+  </si>
+  <si>
+    <t>TFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table fans </t>
   </si>
 </sst>
 </file>
@@ -367,7 +367,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="A3" sqref="A3:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,10 +390,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>

</xml_diff>